<commit_message>
ReportsDailyDetile 7 my condition
</commit_message>
<xml_diff>
--- a/temp/mycondition.xlsx
+++ b/temp/mycondition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mydjango\mojallal24mehr\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8576FF2A-E9A9-4477-9326-A75DAB116A7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA81158D-9571-4CD9-85AE-935553E46641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -406,7 +406,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -457,6 +457,9 @@
       <c r="C2" s="2">
         <v>3</v>
       </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
       <c r="E2" s="2" t="s">
         <v>7</v>
       </c>

</xml_diff>